<commit_message>
atualização dos diagramas da oficina e da locadora
</commit_message>
<xml_diff>
--- a/aula12/tabelas_oficina.xlsx
+++ b/aula12/tabelas_oficina.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aluno.tarde\Desktop\banco_dados_senai\aula12\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C266C734-9A95-4951-B682-787AD85D1A59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F804F320-2665-4F8D-AF95-F3451217D6A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F0599CAF-2E0E-497E-BC89-5308BF40CF4A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="69">
   <si>
     <t>id_cliente</t>
   </si>
@@ -238,6 +238,9 @@
   </si>
   <si>
     <t>tbl_peca</t>
+  </si>
+  <si>
+    <t>tbl_estoque</t>
   </si>
 </sst>
 </file>
@@ -566,7 +569,7 @@
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="61">
+  <dxfs count="67">
     <dxf>
       <font>
         <b val="0"/>
@@ -656,6 +659,101 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -673,101 +771,6 @@
           <color indexed="64"/>
         </horizontal>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -793,6 +796,72 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -806,8 +875,214 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -867,16 +1142,9 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
+    </dxf>
+    <dxf>
+      <border>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -935,21 +1203,201 @@
         <scheme val="none"/>
       </font>
       <fill>
-        <patternFill patternType="none">
+        <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor auto="1"/>
+          <bgColor theme="6" tint="0.39997558519241921"/>
         </patternFill>
       </fill>
-      <alignment horizontal="centerContinuous" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -988,37 +1436,28 @@
       </border>
     </dxf>
     <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
+        <right/>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -1050,7 +1489,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -1090,6 +1529,65 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1116,10 +1614,10 @@
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -1135,6 +1633,55 @@
       </border>
     </dxf>
     <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1152,364 +1699,22 @@
         <scheme val="none"/>
       </font>
       <fill>
-        <patternFill patternType="solid">
+        <patternFill patternType="none">
           <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.59999389629810485"/>
+          <bgColor auto="1"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="centerContinuous" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -2311,7 +2516,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DAF0D619-5B67-497A-9085-0A7D9E3E62DB}" name="Tabela1" displayName="Tabela1" ref="A4:E7" totalsRowShown="0" headerRowDxfId="60" headerRowBorderDxfId="59" tableBorderDxfId="58" totalsRowBorderDxfId="57">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DAF0D619-5B67-497A-9085-0A7D9E3E62DB}" name="Tabela1" displayName="Tabela1" ref="A4:E7" totalsRowShown="0" headerRowDxfId="66" headerRowBorderDxfId="65" tableBorderDxfId="64" totalsRowBorderDxfId="63">
   <autoFilter ref="A4:E7" xr:uid="{DAF0D619-5B67-497A-9085-0A7D9E3E62DB}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -2320,34 +2525,34 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{7FF4384E-1CB7-497F-ABEB-C1D7E12A118F}" name="id_cliente" dataDxfId="56"/>
-    <tableColumn id="2" xr3:uid="{DD759FC9-A8A0-414A-A014-E8F02C5585E5}" name="nome" dataDxfId="55"/>
-    <tableColumn id="3" xr3:uid="{7AAC6059-276F-420B-BE0C-5412D71420FA}" name="CPF" dataDxfId="54"/>
-    <tableColumn id="4" xr3:uid="{C57D034C-1B64-4185-B31D-7C51D0810497}" name="id_endereco_cliente" dataDxfId="53"/>
-    <tableColumn id="5" xr3:uid="{AF008B1E-813C-4F91-A855-F8A3B72CDCCF}" name="id_contato_cliente" dataDxfId="52"/>
+    <tableColumn id="1" xr3:uid="{7FF4384E-1CB7-497F-ABEB-C1D7E12A118F}" name="id_cliente" dataDxfId="62"/>
+    <tableColumn id="2" xr3:uid="{DD759FC9-A8A0-414A-A014-E8F02C5585E5}" name="nome" dataDxfId="61"/>
+    <tableColumn id="3" xr3:uid="{7AAC6059-276F-420B-BE0C-5412D71420FA}" name="CPF" dataDxfId="60"/>
+    <tableColumn id="4" xr3:uid="{C57D034C-1B64-4185-B31D-7C51D0810497}" name="id_endereco_cliente" dataDxfId="59"/>
+    <tableColumn id="5" xr3:uid="{AF008B1E-813C-4F91-A855-F8A3B72CDCCF}" name="id_contato_cliente" dataDxfId="58"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5723CFB0-92B7-4363-B691-27EE97F7526A}" name="Tabela13" displayName="Tabela13" ref="G4:I7" totalsRowShown="0" headerRowDxfId="51" headerRowBorderDxfId="50" tableBorderDxfId="49" totalsRowBorderDxfId="48">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5723CFB0-92B7-4363-B691-27EE97F7526A}" name="Tabela13" displayName="Tabela13" ref="G4:I7" totalsRowShown="0" headerRowDxfId="57" headerRowBorderDxfId="56" tableBorderDxfId="55" totalsRowBorderDxfId="54">
   <autoFilter ref="G4:I7" xr:uid="{5723CFB0-92B7-4363-B691-27EE97F7526A}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{5B8810D7-BADD-45FB-80F0-14657EF2530A}" name="id_contato_cliente" dataDxfId="47"/>
-    <tableColumn id="2" xr3:uid="{B643AB82-3E84-4168-8AF2-77D7D3FF882F}" name="telefone_pessoal" dataDxfId="46"/>
-    <tableColumn id="3" xr3:uid="{C1FF3BA5-34BF-4F65-B563-AEF06371069A}" name="telefone_residencial" dataDxfId="45"/>
+    <tableColumn id="1" xr3:uid="{5B8810D7-BADD-45FB-80F0-14657EF2530A}" name="id_contato_cliente" dataDxfId="53"/>
+    <tableColumn id="2" xr3:uid="{B643AB82-3E84-4168-8AF2-77D7D3FF882F}" name="telefone_pessoal" dataDxfId="52"/>
+    <tableColumn id="3" xr3:uid="{C1FF3BA5-34BF-4F65-B563-AEF06371069A}" name="telefone_residencial" dataDxfId="51"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0AA4C7CB-A969-415E-97BB-1E15651D425F}" name="Tabela3" displayName="Tabela3" ref="K4:R7" totalsRowShown="0" headerRowDxfId="44" dataDxfId="42" headerRowBorderDxfId="43" tableBorderDxfId="41" totalsRowBorderDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0AA4C7CB-A969-415E-97BB-1E15651D425F}" name="Tabela3" displayName="Tabela3" ref="K4:R7" totalsRowShown="0" headerRowDxfId="50" dataDxfId="48" headerRowBorderDxfId="49" tableBorderDxfId="47" totalsRowBorderDxfId="46">
   <autoFilter ref="K4:R7" xr:uid="{0AA4C7CB-A969-415E-97BB-1E15651D425F}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -2359,21 +2564,21 @@
     <filterColumn colId="7" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="8">
-    <tableColumn id="2" xr3:uid="{E0EAE200-4D94-4CAD-B58B-F8F3F17AB389}" name="id_endereco_cliente" dataDxfId="39"/>
-    <tableColumn id="3" xr3:uid="{EA56BBCD-7B12-4B0F-B620-3617F148901B}" name="logradouro" dataDxfId="38"/>
-    <tableColumn id="4" xr3:uid="{618BDE9A-64E6-4031-99DB-9062304D1CC7}" name="numero" dataDxfId="37"/>
-    <tableColumn id="5" xr3:uid="{F9DACAC5-44A6-430C-A543-F8EF065C0621}" name="complemento" dataDxfId="36"/>
-    <tableColumn id="6" xr3:uid="{30206026-7329-4B95-8D0D-7A239A6D6446}" name="bairro" dataDxfId="35"/>
-    <tableColumn id="7" xr3:uid="{28C950F2-8B76-4A74-8890-CCC98DC243A1}" name="cidade" dataDxfId="34"/>
-    <tableColumn id="8" xr3:uid="{9F89E7C7-7C7D-44CF-A5A1-100A1958194D}" name=" uf" dataDxfId="33"/>
-    <tableColumn id="9" xr3:uid="{FA0AEE56-760A-4049-97F8-2F456B4696EF}" name="cep" dataDxfId="32"/>
+    <tableColumn id="2" xr3:uid="{E0EAE200-4D94-4CAD-B58B-F8F3F17AB389}" name="id_endereco_cliente" dataDxfId="45"/>
+    <tableColumn id="3" xr3:uid="{EA56BBCD-7B12-4B0F-B620-3617F148901B}" name="logradouro" dataDxfId="44"/>
+    <tableColumn id="4" xr3:uid="{618BDE9A-64E6-4031-99DB-9062304D1CC7}" name="numero" dataDxfId="43"/>
+    <tableColumn id="5" xr3:uid="{F9DACAC5-44A6-430C-A543-F8EF065C0621}" name="complemento" dataDxfId="42"/>
+    <tableColumn id="6" xr3:uid="{30206026-7329-4B95-8D0D-7A239A6D6446}" name="bairro" dataDxfId="41"/>
+    <tableColumn id="7" xr3:uid="{28C950F2-8B76-4A74-8890-CCC98DC243A1}" name="cidade" dataDxfId="40"/>
+    <tableColumn id="8" xr3:uid="{9F89E7C7-7C7D-44CF-A5A1-100A1958194D}" name=" uf" dataDxfId="39"/>
+    <tableColumn id="9" xr3:uid="{FA0AEE56-760A-4049-97F8-2F456B4696EF}" name="cep" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4994BB7D-AC6C-4244-99A8-D79CD883B245}" name="Tabela4" displayName="Tabela4" ref="A10:E13" totalsRowShown="0" headerRowDxfId="11" dataDxfId="31" headerRowBorderDxfId="28" tableBorderDxfId="29" totalsRowBorderDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4994BB7D-AC6C-4244-99A8-D79CD883B245}" name="Tabela4" displayName="Tabela4" ref="A10:E13" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36" tableBorderDxfId="34" totalsRowBorderDxfId="33">
   <autoFilter ref="A10:E13" xr:uid="{4994BB7D-AC6C-4244-99A8-D79CD883B245}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -2382,18 +2587,18 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{81CCDA74-CE40-49F5-B2D3-7F78A08E3CEF}" name="id_veiculo" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{EB91A0D4-D4BF-4840-924C-C6CFB75C8E70}" name="placa_veiculo" dataDxfId="25"/>
-    <tableColumn id="3" xr3:uid="{3852152B-D3A3-40C3-A59B-1E5BC93C2576}" name="modelo" dataDxfId="24"/>
-    <tableColumn id="4" xr3:uid="{2E801D9E-33B3-4DC1-8473-4E43BFFE89E0}" name="ano" dataDxfId="23"/>
-    <tableColumn id="5" xr3:uid="{A6EC6BD1-C6D0-49E6-9E33-43EC53AECEE3}" name="cor" dataDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{81CCDA74-CE40-49F5-B2D3-7F78A08E3CEF}" name="id_veiculo" dataDxfId="32"/>
+    <tableColumn id="2" xr3:uid="{EB91A0D4-D4BF-4840-924C-C6CFB75C8E70}" name="placa_veiculo" dataDxfId="31"/>
+    <tableColumn id="3" xr3:uid="{3852152B-D3A3-40C3-A59B-1E5BC93C2576}" name="modelo" dataDxfId="30"/>
+    <tableColumn id="4" xr3:uid="{2E801D9E-33B3-4DC1-8473-4E43BFFE89E0}" name="ano" dataDxfId="29"/>
+    <tableColumn id="5" xr3:uid="{A6EC6BD1-C6D0-49E6-9E33-43EC53AECEE3}" name="cor" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A57B934E-742D-4457-83C4-CCC2A010FC52}" name="Tabela5" displayName="Tabela5" ref="G10:J13" totalsRowShown="0" headerRowDxfId="10" dataDxfId="30" headerRowBorderDxfId="20" tableBorderDxfId="21" totalsRowBorderDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A57B934E-742D-4457-83C4-CCC2A010FC52}" name="Tabela5" displayName="Tabela5" ref="G10:J13" totalsRowShown="0" headerRowDxfId="27" dataDxfId="25" headerRowBorderDxfId="26" tableBorderDxfId="24" totalsRowBorderDxfId="23">
   <autoFilter ref="G10:J13" xr:uid="{A57B934E-742D-4457-83C4-CCC2A010FC52}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -2401,17 +2606,17 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{86C30DFF-C6EA-48BA-824C-F5E7D2C1A166}" name="id_cliente_veiculo" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{091198C2-6F5D-4F73-BA8D-401C224024FA}" name="id_cliente" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{8E26C55E-8A31-4DE4-A090-4AAEEFA476AE}" name="id_veiculo" dataDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{6AE8B2DB-4A87-42BD-B000-F260765A188E}" name="cod_servico" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{86C30DFF-C6EA-48BA-824C-F5E7D2C1A166}" name="id_cliente_veiculo" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{091198C2-6F5D-4F73-BA8D-401C224024FA}" name="id_cliente" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{8E26C55E-8A31-4DE4-A090-4AAEEFA476AE}" name="id_veiculo" dataDxfId="20"/>
+    <tableColumn id="4" xr3:uid="{6AE8B2DB-4A87-42BD-B000-F260765A188E}" name="cod_servico" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{2FC9B660-0DE1-4812-BFC7-7551E34153BA}" name="Tabela6" displayName="Tabela6" ref="A16:D19" totalsRowShown="0" headerRowDxfId="9" dataDxfId="15" headerRowBorderDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{2FC9B660-0DE1-4812-BFC7-7551E34153BA}" name="Tabela6" displayName="Tabela6" ref="A16:D19" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17">
   <autoFilter ref="A16:D19" xr:uid="{2FC9B660-0DE1-4812-BFC7-7551E34153BA}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -2419,17 +2624,17 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{234C9F49-A44F-4874-AACE-BF88DE027174}" name="cod_servico" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{D406B339-FDD9-458B-B250-C0004E93A9A6}" name="data" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{ECF2905B-2270-4EE4-BEDC-6D4A25D550B8}" name="nome" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{FEDE2432-5F89-43BB-ACAD-349B35823D14}" name="preco" dataDxfId="13" dataCellStyle="Moeda"/>
+    <tableColumn id="1" xr3:uid="{234C9F49-A44F-4874-AACE-BF88DE027174}" name="cod_servico" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{D406B339-FDD9-458B-B250-C0004E93A9A6}" name="data" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{ECF2905B-2270-4EE4-BEDC-6D4A25D550B8}" name="nome" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{FEDE2432-5F89-43BB-ACAD-349B35823D14}" name="preco" dataDxfId="12" dataCellStyle="Moeda"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{719FA253-C09E-4CB2-B7AF-67BF96E6A768}" name="Tabela7" displayName="Tabela7" ref="G16:J19" totalsRowShown="0" headerRowDxfId="2" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{719FA253-C09E-4CB2-B7AF-67BF96E6A768}" name="Tabela7" displayName="Tabela7" ref="G16:J19" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="G16:J19" xr:uid="{719FA253-C09E-4CB2-B7AF-67BF96E6A768}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -2437,10 +2642,23 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{1136CBAB-D4AD-48B9-9808-914E30AC7EB7}" name="cod_peca" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{AC815401-0DC5-4633-913F-EB387055643A}" name="nome" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{63BAA0DF-B269-451E-9595-2B3DDA158E52}" name="descricao" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{41B30716-4406-44CD-8CE2-FD723B47ECE8}" name="cod_servico" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{1136CBAB-D4AD-48B9-9808-914E30AC7EB7}" name="cod_peca" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{AC815401-0DC5-4633-913F-EB387055643A}" name="nome" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{63BAA0DF-B269-451E-9595-2B3DDA158E52}" name="descricao" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{41B30716-4406-44CD-8CE2-FD723B47ECE8}" name="cod_servico" dataDxfId="6"/>
+  </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{17701990-42E3-4E29-B94F-A9FF382618C4}" name="Tabela79" displayName="Tabela79" ref="L16:O19" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="L16:O19" xr:uid="{17701990-42E3-4E29-B94F-A9FF382618C4}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{01A90589-4DCE-4FA3-970B-6A48D71B1144}" name="cod_peca" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{053E4D2E-17AE-41F1-8790-9D2D69D747EF}" name="nome" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{05B52311-D8C5-4EC0-9249-377AE541A136}" name="descricao" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{E97F0C12-F015-470F-B0DA-24EACABA5DAE}" name="cod_servico" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2746,7 +2964,7 @@
   <dimension ref="A3:R19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="L1" sqref="L1:O1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2762,10 +2980,10 @@
     <col min="9" max="9" width="21.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.140625" style="1" customWidth="1"/>
     <col min="11" max="11" width="23.42578125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="13.85546875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="10.5703125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="16.5703125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="16" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="9.140625" style="1"/>
     <col min="18" max="18" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
@@ -3135,6 +3353,12 @@
       <c r="H15" s="31"/>
       <c r="I15" s="31"/>
       <c r="J15" s="31"/>
+      <c r="L15" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="M15" s="31"/>
+      <c r="N15" s="31"/>
+      <c r="O15" s="31"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="35" t="s">
@@ -3161,8 +3385,20 @@
       <c r="J16" s="37" t="s">
         <v>56</v>
       </c>
+      <c r="L16" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N16" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="O16" s="37" t="s">
+        <v>56</v>
+      </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="36">
         <v>1</v>
       </c>
@@ -3185,8 +3421,18 @@
       <c r="J17" s="36">
         <v>1</v>
       </c>
+      <c r="L17" s="2">
+        <v>1</v>
+      </c>
+      <c r="M17" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="N17" s="3"/>
+      <c r="O17" s="36">
+        <v>1</v>
+      </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="36">
         <v>2</v>
       </c>
@@ -3207,8 +3453,16 @@
       </c>
       <c r="I18" s="3"/>
       <c r="J18" s="36"/>
+      <c r="L18" s="2">
+        <v>2</v>
+      </c>
+      <c r="M18" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="N18" s="3"/>
+      <c r="O18" s="36"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="36">
         <v>3</v>
       </c>
@@ -3229,11 +3483,19 @@
       </c>
       <c r="I19" s="3"/>
       <c r="J19" s="36"/>
+      <c r="L19" s="2">
+        <v>3</v>
+      </c>
+      <c r="M19" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="N19" s="3"/>
+      <c r="O19" s="36"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="7">
+  <tableParts count="8">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
@@ -3241,6 +3503,7 @@
     <tablePart r:id="rId6"/>
     <tablePart r:id="rId7"/>
     <tablePart r:id="rId8"/>
+    <tablePart r:id="rId9"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Atualização dos exercícios da aula 12 e 13
</commit_message>
<xml_diff>
--- a/aula12/tabelas_oficina.xlsx
+++ b/aula12/tabelas_oficina.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aluno.tarde\Desktop\banco_dados_senai\aula12\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F804F320-2665-4F8D-AF95-F3451217D6A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4F40FD7-A910-4A9C-8926-B57056FFF845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F0599CAF-2E0E-497E-BC89-5308BF40CF4A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="73">
   <si>
     <t>id_cliente</t>
   </si>
@@ -241,6 +241,18 @@
   </si>
   <si>
     <t>tbl_estoque</t>
+  </si>
+  <si>
+    <t>id_estoque</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>entrada</t>
+  </si>
+  <si>
+    <t>saida</t>
   </si>
 </sst>
 </file>
@@ -451,7 +463,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -562,6 +574,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -588,9 +603,9 @@
         <scheme val="none"/>
       </font>
       <fill>
-        <patternFill patternType="solid">
+        <patternFill patternType="none">
           <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.39997558519241921"/>
+          <bgColor auto="1"/>
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -626,7 +641,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -659,47 +674,41 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right style="thin">
           <color indexed="64"/>
@@ -710,12 +719,6 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -2655,10 +2658,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{17701990-42E3-4E29-B94F-A9FF382618C4}" name="Tabela79" displayName="Tabela79" ref="L16:O19" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="L16:O19" xr:uid="{17701990-42E3-4E29-B94F-A9FF382618C4}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{01A90589-4DCE-4FA3-970B-6A48D71B1144}" name="cod_peca" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{053E4D2E-17AE-41F1-8790-9D2D69D747EF}" name="nome" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{05B52311-D8C5-4EC0-9249-377AE541A136}" name="descricao" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{E97F0C12-F015-470F-B0DA-24EACABA5DAE}" name="cod_servico" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{01A90589-4DCE-4FA3-970B-6A48D71B1144}" name="id_estoque" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{053E4D2E-17AE-41F1-8790-9D2D69D747EF}" name="total" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{05B52311-D8C5-4EC0-9249-377AE541A136}" name="entrada" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{E97F0C12-F015-470F-B0DA-24EACABA5DAE}" name="saida" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2963,8 +2966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0233BEA5-2C31-498D-9F39-6938066400A9}">
   <dimension ref="A3:R19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:O1048576"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3386,16 +3389,16 @@
         <v>56</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>1</v>
+        <v>70</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="O16" s="37" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
@@ -3424,12 +3427,14 @@
       <c r="L17" s="2">
         <v>1</v>
       </c>
-      <c r="M17" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="N17" s="3"/>
-      <c r="O17" s="36">
-        <v>1</v>
+      <c r="M17" s="2">
+        <v>10</v>
+      </c>
+      <c r="N17" s="2">
+        <v>5</v>
+      </c>
+      <c r="O17" s="38">
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
@@ -3456,11 +3461,15 @@
       <c r="L18" s="2">
         <v>2</v>
       </c>
-      <c r="M18" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="N18" s="3"/>
-      <c r="O18" s="36"/>
+      <c r="M18" s="2">
+        <v>3</v>
+      </c>
+      <c r="N18" s="2">
+        <v>5</v>
+      </c>
+      <c r="O18" s="38">
+        <v>3</v>
+      </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="36">
@@ -3486,11 +3495,9 @@
       <c r="L19" s="2">
         <v>3</v>
       </c>
-      <c r="M19" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="N19" s="3"/>
-      <c r="O19" s="36"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="38"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Finalização da atividade da aula 12
</commit_message>
<xml_diff>
--- a/aula12/tabelas_oficina.xlsx
+++ b/aula12/tabelas_oficina.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aluno.tarde\Desktop\banco_dados_senai\aula12\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fd51511546e56099/Documentos/pasta_001_anderson_de_matos_guimaraes/pasta_01_aulas_e_cursos/pasta-senai/banco_dados_senai/aula12/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4F40FD7-A910-4A9C-8926-B57056FFF845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="128" documentId="13_ncr:1_{D4F40FD7-A910-4A9C-8926-B57056FFF845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{02FD28BE-447F-42B5-A511-AC03D557F15B}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F0599CAF-2E0E-497E-BC89-5308BF40CF4A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="96">
   <si>
     <t>id_cliente</t>
   </si>
@@ -201,9 +201,6 @@
     <t>tbl_veiculo</t>
   </si>
   <si>
-    <t>tbl_cliente_veiculo</t>
-  </si>
-  <si>
     <t>cod_servico</t>
   </si>
   <si>
@@ -253,6 +250,78 @@
   </si>
   <si>
     <t>saida</t>
+  </si>
+  <si>
+    <t>tbl_historico</t>
+  </si>
+  <si>
+    <t>Óleos</t>
+  </si>
+  <si>
+    <t>Insumo</t>
+  </si>
+  <si>
+    <t>tbl_peca_fornecedor</t>
+  </si>
+  <si>
+    <t>id_peca_fornecedor</t>
+  </si>
+  <si>
+    <t>cod_fornecedor</t>
+  </si>
+  <si>
+    <t>tbl_fornecedor</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>nome_representante</t>
+  </si>
+  <si>
+    <t>ABC Peças</t>
+  </si>
+  <si>
+    <t>DEF Peças</t>
+  </si>
+  <si>
+    <t>GHI Peças</t>
+  </si>
+  <si>
+    <t>abc@email.com</t>
+  </si>
+  <si>
+    <t>def@email.com</t>
+  </si>
+  <si>
+    <t>ghi@email.com</t>
+  </si>
+  <si>
+    <t>Andrea Bretas</t>
+  </si>
+  <si>
+    <t>Diego Espíndola</t>
+  </si>
+  <si>
+    <t>Gustavo Holanda</t>
+  </si>
+  <si>
+    <t>tbl_endereco_fornecedor</t>
+  </si>
+  <si>
+    <t>id_endereco_fornecedor</t>
+  </si>
+  <si>
+    <t>tbl_contato_fornecedor</t>
+  </si>
+  <si>
+    <t>id_contato_fornecedor</t>
+  </si>
+  <si>
+    <t>telefone_comercial</t>
+  </si>
+  <si>
+    <t>TABELAS RELACIONAMENTO OFICINA</t>
   </si>
 </sst>
 </file>
@@ -262,7 +331,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -283,8 +352,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -324,6 +400,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -463,7 +569,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -491,9 +597,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -558,16 +661,16 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -576,15 +679,273 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="67">
+  <dxfs count="101">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -641,72 +1002,12 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
@@ -739,25 +1040,45 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="centerContinuous" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -773,6 +1094,792 @@
         <horizontal style="thin">
           <color indexed="64"/>
         </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="centerContinuous" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="centerContinuous" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -864,7 +1971,98 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -872,12 +2070,8 @@
         <right style="thin">
           <color indexed="64"/>
         </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
+        <top/>
+        <bottom/>
         <vertical style="thin">
           <color indexed="64"/>
         </vertical>
@@ -2519,7 +3713,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DAF0D619-5B67-497A-9085-0A7D9E3E62DB}" name="Tabela1" displayName="Tabela1" ref="A4:E7" totalsRowShown="0" headerRowDxfId="66" headerRowBorderDxfId="65" tableBorderDxfId="64" totalsRowBorderDxfId="63">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DAF0D619-5B67-497A-9085-0A7D9E3E62DB}" name="Tabela1" displayName="Tabela1" ref="A4:E7" totalsRowShown="0" headerRowDxfId="100" headerRowBorderDxfId="99" tableBorderDxfId="98" totalsRowBorderDxfId="97">
   <autoFilter ref="A4:E7" xr:uid="{DAF0D619-5B67-497A-9085-0A7D9E3E62DB}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -2528,35 +3722,57 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{7FF4384E-1CB7-497F-ABEB-C1D7E12A118F}" name="id_cliente" dataDxfId="62"/>
-    <tableColumn id="2" xr3:uid="{DD759FC9-A8A0-414A-A014-E8F02C5585E5}" name="nome" dataDxfId="61"/>
-    <tableColumn id="3" xr3:uid="{7AAC6059-276F-420B-BE0C-5412D71420FA}" name="CPF" dataDxfId="60"/>
-    <tableColumn id="4" xr3:uid="{C57D034C-1B64-4185-B31D-7C51D0810497}" name="id_endereco_cliente" dataDxfId="59"/>
-    <tableColumn id="5" xr3:uid="{AF008B1E-813C-4F91-A855-F8A3B72CDCCF}" name="id_contato_cliente" dataDxfId="58"/>
+    <tableColumn id="1" xr3:uid="{7FF4384E-1CB7-497F-ABEB-C1D7E12A118F}" name="id_cliente" dataDxfId="96"/>
+    <tableColumn id="2" xr3:uid="{DD759FC9-A8A0-414A-A014-E8F02C5585E5}" name="nome" dataDxfId="95"/>
+    <tableColumn id="3" xr3:uid="{7AAC6059-276F-420B-BE0C-5412D71420FA}" name="CPF" dataDxfId="94"/>
+    <tableColumn id="4" xr3:uid="{C57D034C-1B64-4185-B31D-7C51D0810497}" name="id_endereco_cliente" dataDxfId="93"/>
+    <tableColumn id="5" xr3:uid="{AF008B1E-813C-4F91-A855-F8A3B72CDCCF}" name="id_contato_cliente" dataDxfId="92"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5723CFB0-92B7-4363-B691-27EE97F7526A}" name="Tabela13" displayName="Tabela13" ref="G4:I7" totalsRowShown="0" headerRowDxfId="57" headerRowBorderDxfId="56" tableBorderDxfId="55" totalsRowBorderDxfId="54">
-  <autoFilter ref="G4:I7" xr:uid="{5723CFB0-92B7-4363-B691-27EE97F7526A}">
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{EA0E553D-D2C6-45B7-BDAF-1EC71BCC1D7E}" name="Tabela61011" displayName="Tabela61011" ref="A58:F61" totalsRowShown="0" headerRowDxfId="9" dataDxfId="32" headerRowBorderDxfId="31">
+  <autoFilter ref="A58:F61" xr:uid="{EA0E553D-D2C6-45B7-BDAF-1EC71BCC1D7E}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{A05B5EAB-8C65-4F59-9B18-FB0E35EA6312}" name="cod_fornecedor" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{18331B68-AB91-475C-B017-BA89939B25CD}" name="nome" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{908C0130-D439-42E0-9805-20448234522B}" name="email" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{DA6BA99E-B554-449C-AF23-967BB58ABCA6}" name="nome_representante" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{2FF3A317-84DD-441C-BC7B-575E5A6670F7}" name="id_contato_fornecedor" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{856DBF3C-F760-4855-B8DD-737E350F287D}" name="id_endereco_fornecedor" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{48C6AF3D-E725-4B9A-94DC-386A1C45AFB7}" name="Tabela61012" displayName="Tabela61012" ref="A64:C67" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28" headerRowBorderDxfId="27">
+  <autoFilter ref="A64:C67" xr:uid="{48C6AF3D-E725-4B9A-94DC-386A1C45AFB7}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{5B8810D7-BADD-45FB-80F0-14657EF2530A}" name="id_contato_cliente" dataDxfId="53"/>
-    <tableColumn id="2" xr3:uid="{B643AB82-3E84-4168-8AF2-77D7D3FF882F}" name="telefone_pessoal" dataDxfId="52"/>
-    <tableColumn id="3" xr3:uid="{C1FF3BA5-34BF-4F65-B563-AEF06371069A}" name="telefone_residencial" dataDxfId="51"/>
+    <tableColumn id="1" xr3:uid="{9357BE5D-D030-429A-B10F-C4477AA6505C}" name="id_contato_fornecedor" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{34D627B8-B818-43CA-B616-6FA9285B57DD}" name="telefone_comercial" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{350AD47C-2CA7-4E3B-B714-F66C9DD177D4}" name="telefone_pessoal" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0AA4C7CB-A969-415E-97BB-1E15651D425F}" name="Tabela3" displayName="Tabela3" ref="K4:R7" totalsRowShown="0" headerRowDxfId="50" dataDxfId="48" headerRowBorderDxfId="49" tableBorderDxfId="47" totalsRowBorderDxfId="46">
-  <autoFilter ref="K4:R7" xr:uid="{0AA4C7CB-A969-415E-97BB-1E15651D425F}">
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{AAF98F0A-76C9-4EC2-9369-92D3AB93D4C7}" name="Tabela313" displayName="Tabela313" ref="A70:H73" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25" headerRowBorderDxfId="23" tableBorderDxfId="24" totalsRowBorderDxfId="22">
+  <autoFilter ref="A70:H73" xr:uid="{AAF98F0A-76C9-4EC2-9369-92D3AB93D4C7}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -2567,22 +3783,64 @@
     <filterColumn colId="7" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="8">
-    <tableColumn id="2" xr3:uid="{E0EAE200-4D94-4CAD-B58B-F8F3F17AB389}" name="id_endereco_cliente" dataDxfId="45"/>
-    <tableColumn id="3" xr3:uid="{EA56BBCD-7B12-4B0F-B620-3617F148901B}" name="logradouro" dataDxfId="44"/>
-    <tableColumn id="4" xr3:uid="{618BDE9A-64E6-4031-99DB-9062304D1CC7}" name="numero" dataDxfId="43"/>
-    <tableColumn id="5" xr3:uid="{F9DACAC5-44A6-430C-A543-F8EF065C0621}" name="complemento" dataDxfId="42"/>
-    <tableColumn id="6" xr3:uid="{30206026-7329-4B95-8D0D-7A239A6D6446}" name="bairro" dataDxfId="41"/>
-    <tableColumn id="7" xr3:uid="{28C950F2-8B76-4A74-8890-CCC98DC243A1}" name="cidade" dataDxfId="40"/>
-    <tableColumn id="8" xr3:uid="{9F89E7C7-7C7D-44CF-A5A1-100A1958194D}" name=" uf" dataDxfId="39"/>
-    <tableColumn id="9" xr3:uid="{FA0AEE56-760A-4049-97F8-2F456B4696EF}" name="cep" dataDxfId="38"/>
+    <tableColumn id="2" xr3:uid="{6C2706D5-C102-4673-BDE7-BE47AFD7F6C6}" name="id_endereco_fornecedor" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{150E978A-EF44-4FB1-AF1E-A3B73351E73D}" name="logradouro" dataDxfId="20"/>
+    <tableColumn id="4" xr3:uid="{066BD148-697E-4836-A74A-0A2375F9E63E}" name="numero" dataDxfId="19"/>
+    <tableColumn id="5" xr3:uid="{4D6BBAC9-FC21-4A0E-A7BE-0765521D1F2E}" name="complemento" dataDxfId="18"/>
+    <tableColumn id="6" xr3:uid="{A1143E49-8501-4DE6-9D69-F20B0C5A7131}" name="bairro" dataDxfId="17"/>
+    <tableColumn id="7" xr3:uid="{98F3991F-B5D3-4F92-B33C-24E5E7FF840E}" name="cidade" dataDxfId="16"/>
+    <tableColumn id="8" xr3:uid="{5E9D9B67-ECEF-4AC0-B219-F8567D13368C}" name=" uf" dataDxfId="15"/>
+    <tableColumn id="9" xr3:uid="{060A5DFC-FC4E-4652-AB81-D58F662EAE72}" name="cep" dataDxfId="14"/>
+  </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5723CFB0-92B7-4363-B691-27EE97F7526A}" name="Tabela13" displayName="Tabela13" ref="A10:C13" totalsRowShown="0" headerRowDxfId="91" headerRowBorderDxfId="90" tableBorderDxfId="89" totalsRowBorderDxfId="88">
+  <autoFilter ref="A10:C13" xr:uid="{5723CFB0-92B7-4363-B691-27EE97F7526A}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{5B8810D7-BADD-45FB-80F0-14657EF2530A}" name="id_contato_cliente" dataDxfId="87"/>
+    <tableColumn id="2" xr3:uid="{B643AB82-3E84-4168-8AF2-77D7D3FF882F}" name="telefone_pessoal" dataDxfId="86"/>
+    <tableColumn id="3" xr3:uid="{C1FF3BA5-34BF-4F65-B563-AEF06371069A}" name="telefone_residencial" dataDxfId="85"/>
+  </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0AA4C7CB-A969-415E-97BB-1E15651D425F}" name="Tabela3" displayName="Tabela3" ref="A16:H19" totalsRowShown="0" headerRowDxfId="84" dataDxfId="82" headerRowBorderDxfId="83" tableBorderDxfId="81" totalsRowBorderDxfId="80">
+  <autoFilter ref="A16:H19" xr:uid="{0AA4C7CB-A969-415E-97BB-1E15651D425F}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+    <filterColumn colId="6" hiddenButton="1"/>
+    <filterColumn colId="7" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="8">
+    <tableColumn id="2" xr3:uid="{E0EAE200-4D94-4CAD-B58B-F8F3F17AB389}" name="id_endereco_cliente" dataDxfId="79"/>
+    <tableColumn id="3" xr3:uid="{EA56BBCD-7B12-4B0F-B620-3617F148901B}" name="logradouro" dataDxfId="78"/>
+    <tableColumn id="4" xr3:uid="{618BDE9A-64E6-4031-99DB-9062304D1CC7}" name="numero" dataDxfId="77"/>
+    <tableColumn id="5" xr3:uid="{F9DACAC5-44A6-430C-A543-F8EF065C0621}" name="complemento" dataDxfId="76"/>
+    <tableColumn id="6" xr3:uid="{30206026-7329-4B95-8D0D-7A239A6D6446}" name="bairro" dataDxfId="75"/>
+    <tableColumn id="7" xr3:uid="{28C950F2-8B76-4A74-8890-CCC98DC243A1}" name="cidade" dataDxfId="74"/>
+    <tableColumn id="8" xr3:uid="{9F89E7C7-7C7D-44CF-A5A1-100A1958194D}" name=" uf" dataDxfId="73"/>
+    <tableColumn id="9" xr3:uid="{FA0AEE56-760A-4049-97F8-2F456B4696EF}" name="cep" dataDxfId="72"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4994BB7D-AC6C-4244-99A8-D79CD883B245}" name="Tabela4" displayName="Tabela4" ref="A10:E13" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36" tableBorderDxfId="34" totalsRowBorderDxfId="33">
-  <autoFilter ref="A10:E13" xr:uid="{4994BB7D-AC6C-4244-99A8-D79CD883B245}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4994BB7D-AC6C-4244-99A8-D79CD883B245}" name="Tabela4" displayName="Tabela4" ref="A22:E25" totalsRowShown="0" headerRowDxfId="71" dataDxfId="69" headerRowBorderDxfId="70" tableBorderDxfId="68" totalsRowBorderDxfId="67">
+  <autoFilter ref="A22:E25" xr:uid="{4994BB7D-AC6C-4244-99A8-D79CD883B245}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -2590,87 +3848,108 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{81CCDA74-CE40-49F5-B2D3-7F78A08E3CEF}" name="id_veiculo" dataDxfId="32"/>
-    <tableColumn id="2" xr3:uid="{EB91A0D4-D4BF-4840-924C-C6CFB75C8E70}" name="placa_veiculo" dataDxfId="31"/>
-    <tableColumn id="3" xr3:uid="{3852152B-D3A3-40C3-A59B-1E5BC93C2576}" name="modelo" dataDxfId="30"/>
-    <tableColumn id="4" xr3:uid="{2E801D9E-33B3-4DC1-8473-4E43BFFE89E0}" name="ano" dataDxfId="29"/>
-    <tableColumn id="5" xr3:uid="{A6EC6BD1-C6D0-49E6-9E33-43EC53AECEE3}" name="cor" dataDxfId="28"/>
+    <tableColumn id="1" xr3:uid="{81CCDA74-CE40-49F5-B2D3-7F78A08E3CEF}" name="id_veiculo" dataDxfId="66"/>
+    <tableColumn id="2" xr3:uid="{EB91A0D4-D4BF-4840-924C-C6CFB75C8E70}" name="placa_veiculo" dataDxfId="65"/>
+    <tableColumn id="3" xr3:uid="{3852152B-D3A3-40C3-A59B-1E5BC93C2576}" name="modelo" dataDxfId="64"/>
+    <tableColumn id="4" xr3:uid="{2E801D9E-33B3-4DC1-8473-4E43BFFE89E0}" name="ano" dataDxfId="63"/>
+    <tableColumn id="5" xr3:uid="{A6EC6BD1-C6D0-49E6-9E33-43EC53AECEE3}" name="cor" dataDxfId="62"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A57B934E-742D-4457-83C4-CCC2A010FC52}" name="Tabela5" displayName="Tabela5" ref="G10:J13" totalsRowShown="0" headerRowDxfId="27" dataDxfId="25" headerRowBorderDxfId="26" tableBorderDxfId="24" totalsRowBorderDxfId="23">
-  <autoFilter ref="G10:J13" xr:uid="{A57B934E-742D-4457-83C4-CCC2A010FC52}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A57B934E-742D-4457-83C4-CCC2A010FC52}" name="Tabela5" displayName="Tabela5" ref="A28:D31" totalsRowShown="0" headerRowDxfId="61" dataDxfId="59" headerRowBorderDxfId="60" tableBorderDxfId="58" totalsRowBorderDxfId="57">
+  <autoFilter ref="A28:D31" xr:uid="{A57B934E-742D-4457-83C4-CCC2A010FC52}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{86C30DFF-C6EA-48BA-824C-F5E7D2C1A166}" name="id_cliente_veiculo" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{091198C2-6F5D-4F73-BA8D-401C224024FA}" name="id_cliente" dataDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{8E26C55E-8A31-4DE4-A090-4AAEEFA476AE}" name="id_veiculo" dataDxfId="20"/>
-    <tableColumn id="4" xr3:uid="{6AE8B2DB-4A87-42BD-B000-F260765A188E}" name="cod_servico" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{86C30DFF-C6EA-48BA-824C-F5E7D2C1A166}" name="id_cliente_veiculo" dataDxfId="56"/>
+    <tableColumn id="2" xr3:uid="{091198C2-6F5D-4F73-BA8D-401C224024FA}" name="id_cliente" dataDxfId="55"/>
+    <tableColumn id="3" xr3:uid="{8E26C55E-8A31-4DE4-A090-4AAEEFA476AE}" name="id_veiculo" dataDxfId="54"/>
+    <tableColumn id="4" xr3:uid="{6AE8B2DB-4A87-42BD-B000-F260765A188E}" name="cod_servico" dataDxfId="53"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{2FC9B660-0DE1-4812-BFC7-7551E34153BA}" name="Tabela6" displayName="Tabela6" ref="A16:D19" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17">
-  <autoFilter ref="A16:D19" xr:uid="{2FC9B660-0DE1-4812-BFC7-7551E34153BA}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{2FC9B660-0DE1-4812-BFC7-7551E34153BA}" name="Tabela6" displayName="Tabela6" ref="A34:D37" totalsRowShown="0" headerRowDxfId="52" dataDxfId="50" headerRowBorderDxfId="51">
+  <autoFilter ref="A34:D37" xr:uid="{2FC9B660-0DE1-4812-BFC7-7551E34153BA}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{234C9F49-A44F-4874-AACE-BF88DE027174}" name="cod_servico" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{D406B339-FDD9-458B-B250-C0004E93A9A6}" name="data" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{ECF2905B-2270-4EE4-BEDC-6D4A25D550B8}" name="nome" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{FEDE2432-5F89-43BB-ACAD-349B35823D14}" name="preco" dataDxfId="12" dataCellStyle="Moeda"/>
+    <tableColumn id="1" xr3:uid="{234C9F49-A44F-4874-AACE-BF88DE027174}" name="cod_servico" dataDxfId="49"/>
+    <tableColumn id="2" xr3:uid="{D406B339-FDD9-458B-B250-C0004E93A9A6}" name="data" dataDxfId="48"/>
+    <tableColumn id="3" xr3:uid="{ECF2905B-2270-4EE4-BEDC-6D4A25D550B8}" name="nome" dataDxfId="47"/>
+    <tableColumn id="4" xr3:uid="{FEDE2432-5F89-43BB-ACAD-349B35823D14}" name="preco" dataDxfId="46" dataCellStyle="Moeda"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{719FA253-C09E-4CB2-B7AF-67BF96E6A768}" name="Tabela7" displayName="Tabela7" ref="G16:J19" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="G16:J19" xr:uid="{719FA253-C09E-4CB2-B7AF-67BF96E6A768}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{719FA253-C09E-4CB2-B7AF-67BF96E6A768}" name="Tabela7" displayName="Tabela7" ref="A40:D43" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44">
+  <autoFilter ref="A40:D43" xr:uid="{719FA253-C09E-4CB2-B7AF-67BF96E6A768}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{1136CBAB-D4AD-48B9-9808-914E30AC7EB7}" name="cod_peca" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{AC815401-0DC5-4633-913F-EB387055643A}" name="nome" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{63BAA0DF-B269-451E-9595-2B3DDA158E52}" name="descricao" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{41B30716-4406-44CD-8CE2-FD723B47ECE8}" name="cod_servico" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{1136CBAB-D4AD-48B9-9808-914E30AC7EB7}" name="cod_peca" dataDxfId="43"/>
+    <tableColumn id="2" xr3:uid="{AC815401-0DC5-4633-913F-EB387055643A}" name="nome" dataDxfId="38"/>
+    <tableColumn id="3" xr3:uid="{63BAA0DF-B269-451E-9595-2B3DDA158E52}" name="descricao" dataDxfId="36"/>
+    <tableColumn id="4" xr3:uid="{41B30716-4406-44CD-8CE2-FD723B47ECE8}" name="cod_servico" dataDxfId="37"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{17701990-42E3-4E29-B94F-A9FF382618C4}" name="Tabela79" displayName="Tabela79" ref="L16:O19" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="L16:O19" xr:uid="{17701990-42E3-4E29-B94F-A9FF382618C4}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{17701990-42E3-4E29-B94F-A9FF382618C4}" name="Tabela79" displayName="Tabela79" ref="A46:D49" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
+  <autoFilter ref="A46:D49" xr:uid="{17701990-42E3-4E29-B94F-A9FF382618C4}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+  </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{01A90589-4DCE-4FA3-970B-6A48D71B1144}" name="id_estoque" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{053E4D2E-17AE-41F1-8790-9D2D69D747EF}" name="total" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{05B52311-D8C5-4EC0-9249-377AE541A136}" name="entrada" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{E97F0C12-F015-470F-B0DA-24EACABA5DAE}" name="saida" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{01A90589-4DCE-4FA3-970B-6A48D71B1144}" name="id_estoque" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{053E4D2E-17AE-41F1-8790-9D2D69D747EF}" name="total" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{05B52311-D8C5-4EC0-9249-377AE541A136}" name="entrada" dataDxfId="40"/>
+    <tableColumn id="4" xr3:uid="{E97F0C12-F015-470F-B0DA-24EACABA5DAE}" name="saida" dataDxfId="39"/>
+  </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{063C8D7A-1619-488D-BC11-F8515FD673F8}" name="Tabela610" displayName="Tabela610" ref="A52:C55" totalsRowShown="0" headerRowDxfId="33" dataDxfId="35" headerRowBorderDxfId="34">
+  <autoFilter ref="A52:C55" xr:uid="{063C8D7A-1619-488D-BC11-F8515FD673F8}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{5E019497-35FC-4EC0-A1D3-949EB3D621DD}" name="id_peca_fornecedor" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{CC9DAD04-3656-4CB8-ADF2-BD860460B1EC}" name="cod_peca" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{B5CEB886-B281-4EAB-BBF1-6CB137EFADDF}" name="cod_fornecedor" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2708,7 +3987,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2814,7 +4093,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2956,7 +4235,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2964,60 +4243,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0233BEA5-2C31-498D-9F39-6938066400A9}">
-  <dimension ref="A3:R19"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:H75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="22" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="1"/>
-    <col min="7" max="7" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.85546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="21.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="23.42578125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.140625" style="1"/>
-    <col min="18" max="18" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="26.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="31" t="s">
+    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A1" s="49" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="G3" s="31" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3" s="31"/>
-      <c r="I3" s="31"/>
-      <c r="K3" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="L3" s="31"/>
-      <c r="M3" s="31"/>
-      <c r="N3" s="31"/>
-      <c r="O3" s="31"/>
-      <c r="P3" s="31"/>
-      <c r="Q3" s="31"/>
-      <c r="R3" s="31"/>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>0</v>
       </c>
@@ -3033,42 +4300,9 @@
       <c r="E4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="M4" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="N4" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="O4" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="P4" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q4" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="R4" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="12">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="11">
         <v>1</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -3077,46 +4311,15 @@
       <c r="C5" s="4">
         <v>12345678910</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="13">
         <v>1</v>
       </c>
-      <c r="E5" s="16">
+      <c r="E5" s="15">
         <v>1</v>
       </c>
-      <c r="G5" s="14">
-        <v>1</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K5" s="16">
-        <v>1</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="M5" s="2">
-        <v>100</v>
-      </c>
-      <c r="N5" s="2"/>
-      <c r="O5" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="P5" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q5" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="R5" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="12">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="11">
         <v>2</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -3125,46 +4328,15 @@
       <c r="C6" s="4">
         <v>98765432101</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="13">
         <v>2</v>
       </c>
-      <c r="E6" s="16">
+      <c r="E6" s="15">
         <v>2</v>
       </c>
-      <c r="G6" s="14">
-        <v>2</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="K6" s="16">
-        <v>2</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="M6" s="2">
-        <v>101</v>
-      </c>
-      <c r="N6" s="2"/>
-      <c r="O6" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="P6" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q6" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="R6" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="13">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="12">
         <v>3</v>
       </c>
       <c r="B7" s="8" t="s">
@@ -3173,336 +4345,1066 @@
       <c r="C7" s="9">
         <v>15975318300</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D7" s="13">
         <v>3</v>
       </c>
-      <c r="E7" s="16">
+      <c r="E7" s="15">
         <v>3</v>
       </c>
-      <c r="G7" s="15">
+    </row>
+    <row r="8" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="43"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
+    </row>
+    <row r="9" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="43"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="43"/>
+    </row>
+    <row r="10" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="G10" s="43"/>
+      <c r="H10" s="43"/>
+    </row>
+    <row r="11" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="13">
+        <v>1</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="43"/>
+    </row>
+    <row r="12" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="13">
+        <v>2</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="43"/>
+      <c r="E12" s="43"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="43"/>
+    </row>
+    <row r="13" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="14">
         <v>3</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="B13" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="9" t="s">
+      <c r="C13" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="K7" s="17">
+      <c r="D13" s="43"/>
+      <c r="E13" s="43"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="43"/>
+    </row>
+    <row r="14" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="43"/>
+      <c r="B14" s="44"/>
+      <c r="C14" s="43"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="43"/>
+      <c r="G14" s="43"/>
+      <c r="H14" s="43"/>
+    </row>
+    <row r="15" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="30"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
+    </row>
+    <row r="16" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="15">
+        <v>1</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="2">
+        <v>100</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="15">
+        <v>2</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="2">
+        <v>101</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="16">
         <v>3</v>
       </c>
-      <c r="L7" s="8" t="s">
+      <c r="B19" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="M7" s="11">
+      <c r="C19" s="10">
         <v>102</v>
       </c>
-      <c r="N7" s="11"/>
-      <c r="O7" s="8" t="s">
+      <c r="D19" s="10"/>
+      <c r="E19" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="P7" s="8" t="s">
+      <c r="F19" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="Q7" s="11" t="s">
+      <c r="G19" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="R7" s="9" t="s">
+      <c r="H19" s="9" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="31" t="s">
+    <row r="20" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="43"/>
+      <c r="B20" s="44"/>
+      <c r="C20" s="43"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="43"/>
+      <c r="G20" s="43"/>
+      <c r="H20" s="43"/>
+    </row>
+    <row r="21" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="B9" s="31"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="18" t="s">
+      <c r="B21" s="30"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
+      <c r="G21" s="43"/>
+      <c r="H21" s="43"/>
+    </row>
+    <row r="22" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="E22" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="G22" s="43"/>
+      <c r="H22" s="43"/>
+    </row>
+    <row r="23" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="18">
+        <v>1</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="2">
+        <v>2021</v>
+      </c>
+      <c r="D23" s="2">
+        <v>2021</v>
+      </c>
+      <c r="E23" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="G23" s="43"/>
+      <c r="H23" s="43"/>
+    </row>
+    <row r="24" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="18">
+        <v>2</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="2">
+        <v>2020</v>
+      </c>
+      <c r="D24" s="2">
+        <v>2020</v>
+      </c>
+      <c r="E24" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="G24" s="43"/>
+      <c r="H24" s="43"/>
+    </row>
+    <row r="25" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="20">
+        <v>3</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="10">
+        <v>2022</v>
+      </c>
+      <c r="D25" s="10">
+        <v>2022</v>
+      </c>
+      <c r="E25" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="G25" s="43"/>
+      <c r="H25" s="43"/>
+    </row>
+    <row r="26" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="43"/>
+      <c r="B26" s="44"/>
+      <c r="C26" s="43"/>
+      <c r="D26" s="43"/>
+      <c r="E26" s="43"/>
+      <c r="G26" s="43"/>
+      <c r="H26" s="43"/>
+    </row>
+    <row r="27" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="B27" s="17"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="43"/>
+      <c r="G27" s="43"/>
+      <c r="H27" s="43"/>
+    </row>
+    <row r="28" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="D28" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="32" t="s">
-        <v>42</v>
-      </c>
-      <c r="B10" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="C10" s="33" t="s">
+      <c r="E28" s="43"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="43"/>
+    </row>
+    <row r="29" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="22">
+        <v>1</v>
+      </c>
+      <c r="B29" s="23">
+        <v>1</v>
+      </c>
+      <c r="C29" s="24">
+        <v>1</v>
+      </c>
+      <c r="D29" s="35">
+        <v>1</v>
+      </c>
+      <c r="E29" s="43"/>
+      <c r="G29" s="43"/>
+      <c r="H29" s="43"/>
+    </row>
+    <row r="30" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="22">
+        <v>2</v>
+      </c>
+      <c r="B30" s="23">
+        <v>1</v>
+      </c>
+      <c r="C30" s="24">
+        <v>2</v>
+      </c>
+      <c r="D30" s="35">
+        <v>2</v>
+      </c>
+      <c r="E30" s="43"/>
+      <c r="G30" s="43"/>
+      <c r="H30" s="43"/>
+    </row>
+    <row r="31" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="25">
+        <v>3</v>
+      </c>
+      <c r="B31" s="26">
+        <v>3</v>
+      </c>
+      <c r="C31" s="27">
+        <v>2</v>
+      </c>
+      <c r="D31" s="35">
+        <v>3</v>
+      </c>
+      <c r="E31" s="43"/>
+      <c r="G31" s="43"/>
+      <c r="H31" s="43"/>
+    </row>
+    <row r="32" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="43"/>
+      <c r="B32" s="44"/>
+      <c r="C32" s="43"/>
+      <c r="D32" s="43"/>
+      <c r="E32" s="43"/>
+      <c r="G32" s="43"/>
+      <c r="H32" s="43"/>
+    </row>
+    <row r="33" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" s="30"/>
+      <c r="C33" s="30"/>
+      <c r="D33" s="30"/>
+      <c r="E33" s="43"/>
+      <c r="G33" s="43"/>
+      <c r="H33" s="43"/>
+    </row>
+    <row r="34" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="B34" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="C34" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="D34" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="E34" s="43"/>
+      <c r="G34" s="43"/>
+      <c r="H34" s="43"/>
+    </row>
+    <row r="35" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="35">
+        <v>1</v>
+      </c>
+      <c r="B35" s="28">
+        <v>45597</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D35" s="29">
+        <v>30</v>
+      </c>
+      <c r="E35" s="43"/>
+      <c r="G35" s="43"/>
+      <c r="H35" s="43"/>
+    </row>
+    <row r="36" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="35">
+        <v>2</v>
+      </c>
+      <c r="B36" s="28">
+        <v>45598</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D36" s="29">
         <v>45</v>
       </c>
-      <c r="D10" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="E10" s="34" t="s">
-        <v>47</v>
-      </c>
-      <c r="G10" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="H10" s="33" t="s">
+      <c r="E36" s="43"/>
+      <c r="G36" s="43"/>
+      <c r="H36" s="43"/>
+    </row>
+    <row r="37" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="35">
+        <v>3</v>
+      </c>
+      <c r="B37" s="28">
+        <v>45600</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D37" s="29">
+        <v>110</v>
+      </c>
+      <c r="E37" s="43"/>
+      <c r="G37" s="43"/>
+      <c r="H37" s="43"/>
+    </row>
+    <row r="38" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="43"/>
+      <c r="B38" s="44"/>
+      <c r="C38" s="43"/>
+      <c r="D38" s="43"/>
+      <c r="E38" s="43"/>
+      <c r="G38" s="43"/>
+      <c r="H38" s="43"/>
+    </row>
+    <row r="39" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="B39" s="30"/>
+      <c r="C39" s="30"/>
+      <c r="D39" s="30"/>
+      <c r="E39" s="43"/>
+      <c r="G39" s="43"/>
+      <c r="H39" s="43"/>
+    </row>
+    <row r="40" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D40" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="E40" s="43"/>
+      <c r="G40" s="43"/>
+      <c r="H40" s="43"/>
+    </row>
+    <row r="41" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="39">
+        <v>1</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C41" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="D41" s="35">
+        <v>1</v>
+      </c>
+      <c r="E41" s="43"/>
+      <c r="G41" s="43"/>
+      <c r="H41" s="43"/>
+    </row>
+    <row r="42" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="39">
+        <v>2</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C42" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="D42" s="35"/>
+      <c r="E42" s="43"/>
+      <c r="G42" s="43"/>
+      <c r="H42" s="43"/>
+    </row>
+    <row r="43" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="39">
+        <v>3</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C43" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="D43" s="35"/>
+      <c r="E43" s="43"/>
+      <c r="G43" s="43"/>
+      <c r="H43" s="43"/>
+    </row>
+    <row r="44" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="43"/>
+      <c r="B44" s="44"/>
+      <c r="C44" s="43"/>
+      <c r="D44" s="43"/>
+      <c r="E44" s="43"/>
+      <c r="G44" s="43"/>
+      <c r="H44" s="43"/>
+    </row>
+    <row r="45" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="B45" s="30"/>
+      <c r="C45" s="30"/>
+      <c r="D45" s="30"/>
+      <c r="E45" s="43"/>
+      <c r="G45" s="43"/>
+      <c r="H45" s="43"/>
+    </row>
+    <row r="46" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D46" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="E46" s="43"/>
+      <c r="G46" s="43"/>
+      <c r="H46" s="43"/>
+    </row>
+    <row r="47" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="46">
+        <v>1</v>
+      </c>
+      <c r="B47" s="2">
+        <v>10</v>
+      </c>
+      <c r="C47" s="2">
+        <v>5</v>
+      </c>
+      <c r="D47" s="2">
+        <v>5</v>
+      </c>
+      <c r="E47" s="43"/>
+      <c r="G47" s="43"/>
+      <c r="H47" s="43"/>
+    </row>
+    <row r="48" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="46">
+        <v>2</v>
+      </c>
+      <c r="B48" s="2">
+        <v>3</v>
+      </c>
+      <c r="C48" s="2">
+        <v>5</v>
+      </c>
+      <c r="D48" s="2">
+        <v>3</v>
+      </c>
+      <c r="E48" s="43"/>
+      <c r="G48" s="43"/>
+      <c r="H48" s="43"/>
+    </row>
+    <row r="49" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="46">
+        <v>3</v>
+      </c>
+      <c r="B49" s="2">
+        <v>2</v>
+      </c>
+      <c r="C49" s="2">
+        <v>2</v>
+      </c>
+      <c r="D49" s="2">
         <v>0</v>
       </c>
-      <c r="I10" s="34" t="s">
-        <v>42</v>
-      </c>
-      <c r="J10" s="33" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="19">
+      <c r="E49" s="43"/>
+      <c r="G49" s="43"/>
+      <c r="H49" s="43"/>
+    </row>
+    <row r="50" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="43"/>
+      <c r="B50" s="44"/>
+      <c r="C50" s="43"/>
+      <c r="D50" s="43"/>
+      <c r="E50" s="43"/>
+      <c r="G50" s="43"/>
+      <c r="H50" s="43"/>
+    </row>
+    <row r="51" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="B51" s="30"/>
+      <c r="C51" s="30"/>
+      <c r="D51" s="43"/>
+      <c r="E51" s="43"/>
+      <c r="G51" s="43"/>
+      <c r="H51" s="43"/>
+    </row>
+    <row r="52" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C52" s="34" t="s">
+        <v>77</v>
+      </c>
+      <c r="D52" s="43"/>
+      <c r="E52" s="43"/>
+      <c r="G52" s="43"/>
+      <c r="H52" s="43"/>
+    </row>
+    <row r="53" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="48">
         <v>1</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C11" s="2">
-        <v>2021</v>
-      </c>
-      <c r="D11" s="2">
-        <v>2021</v>
-      </c>
-      <c r="E11" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="G11" s="23">
+      <c r="B53" s="39">
         <v>1</v>
       </c>
-      <c r="H11" s="24">
+      <c r="C53" s="42">
         <v>1</v>
       </c>
-      <c r="I11" s="25">
+      <c r="D53" s="43"/>
+      <c r="E53" s="43"/>
+      <c r="G53" s="43"/>
+      <c r="H53" s="43"/>
+    </row>
+    <row r="54" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="48">
+        <v>2</v>
+      </c>
+      <c r="B54" s="39">
+        <v>2</v>
+      </c>
+      <c r="C54" s="42">
+        <v>2</v>
+      </c>
+      <c r="D54" s="43"/>
+      <c r="E54" s="43"/>
+      <c r="G54" s="43"/>
+      <c r="H54" s="43"/>
+    </row>
+    <row r="55" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="48">
+        <v>3</v>
+      </c>
+      <c r="B55" s="39">
+        <v>3</v>
+      </c>
+      <c r="C55" s="42">
+        <v>3</v>
+      </c>
+      <c r="D55" s="43"/>
+      <c r="E55" s="43"/>
+      <c r="G55" s="43"/>
+      <c r="H55" s="43"/>
+    </row>
+    <row r="56" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="43"/>
+      <c r="B56" s="44"/>
+      <c r="C56" s="43"/>
+      <c r="D56" s="43"/>
+      <c r="E56" s="43"/>
+      <c r="G56" s="43"/>
+      <c r="H56" s="43"/>
+    </row>
+    <row r="57" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="B57" s="30"/>
+      <c r="C57" s="30"/>
+      <c r="D57" s="30"/>
+      <c r="E57" s="30"/>
+      <c r="F57" s="30"/>
+      <c r="G57" s="43"/>
+      <c r="H57" s="43"/>
+    </row>
+    <row r="58" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="34" t="s">
+        <v>77</v>
+      </c>
+      <c r="B58" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J11" s="36">
+      <c r="C58" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="D58" s="40" t="s">
+        <v>80</v>
+      </c>
+      <c r="E58" s="40" t="s">
+        <v>93</v>
+      </c>
+      <c r="F58" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="G58" s="43"/>
+      <c r="H58" s="43"/>
+    </row>
+    <row r="59" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="42">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="19">
+      <c r="B59" s="38" t="s">
+        <v>81</v>
+      </c>
+      <c r="C59" s="41" t="s">
+        <v>84</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E59" s="47">
+        <v>1</v>
+      </c>
+      <c r="F59" s="15">
+        <v>1</v>
+      </c>
+      <c r="G59" s="43"/>
+      <c r="H59" s="43"/>
+    </row>
+    <row r="60" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="42">
         <v>2</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C12" s="2">
-        <v>2020</v>
-      </c>
-      <c r="D12" s="2">
-        <v>2020</v>
-      </c>
-      <c r="E12" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="G12" s="23">
+      <c r="B60" s="38" t="s">
+        <v>82</v>
+      </c>
+      <c r="C60" s="41" t="s">
+        <v>85</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E60" s="47">
         <v>2</v>
       </c>
-      <c r="H12" s="24">
+      <c r="F60" s="15">
+        <v>2</v>
+      </c>
+      <c r="G60" s="43"/>
+      <c r="H60" s="43"/>
+    </row>
+    <row r="61" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="42">
+        <v>3</v>
+      </c>
+      <c r="B61" s="38" t="s">
+        <v>83</v>
+      </c>
+      <c r="C61" s="41" t="s">
+        <v>86</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E61" s="47">
+        <v>3</v>
+      </c>
+      <c r="F61" s="15">
+        <v>3</v>
+      </c>
+      <c r="G61" s="43"/>
+      <c r="H61" s="43"/>
+    </row>
+    <row r="62" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="43"/>
+      <c r="B62" s="44"/>
+      <c r="C62" s="43"/>
+      <c r="D62" s="43"/>
+      <c r="E62" s="43"/>
+      <c r="G62" s="43"/>
+      <c r="H62" s="43"/>
+    </row>
+    <row r="63" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="30" t="s">
+        <v>92</v>
+      </c>
+      <c r="B63" s="30"/>
+      <c r="C63" s="30"/>
+      <c r="D63" s="43"/>
+      <c r="E63" s="43"/>
+      <c r="G63" s="43"/>
+      <c r="H63" s="43"/>
+    </row>
+    <row r="64" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="34" t="s">
+        <v>93</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C64" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="D64" s="43"/>
+      <c r="E64" s="43"/>
+      <c r="G64" s="43"/>
+      <c r="H64" s="43"/>
+    </row>
+    <row r="65" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="47">
         <v>1</v>
       </c>
-      <c r="I12" s="25">
+      <c r="B65" s="38">
+        <v>1</v>
+      </c>
+      <c r="C65" s="38">
+        <v>1</v>
+      </c>
+      <c r="D65" s="43"/>
+      <c r="E65" s="43"/>
+      <c r="G65" s="43"/>
+      <c r="H65" s="43"/>
+    </row>
+    <row r="66" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="47">
         <v>2</v>
       </c>
-      <c r="J12" s="36">
+      <c r="B66" s="38">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="21">
+      <c r="C66" s="38">
+        <v>2</v>
+      </c>
+      <c r="D66" s="43"/>
+      <c r="E66" s="43"/>
+      <c r="G66" s="43"/>
+      <c r="H66" s="43"/>
+    </row>
+    <row r="67" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="47">
         <v>3</v>
       </c>
-      <c r="B13" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="C13" s="11">
-        <v>2022</v>
-      </c>
-      <c r="D13" s="11">
-        <v>2022</v>
-      </c>
-      <c r="E13" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="G13" s="26">
+      <c r="B67" s="38">
         <v>3</v>
       </c>
-      <c r="H13" s="27">
+      <c r="C67" s="38">
         <v>3</v>
       </c>
-      <c r="I13" s="28">
+      <c r="D67" s="43"/>
+      <c r="E67" s="43"/>
+      <c r="G67" s="43"/>
+      <c r="H67" s="43"/>
+    </row>
+    <row r="68" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="43"/>
+      <c r="B68" s="44"/>
+      <c r="C68" s="43"/>
+      <c r="D68" s="43"/>
+      <c r="E68" s="43"/>
+      <c r="G68" s="43"/>
+      <c r="H68" s="43"/>
+    </row>
+    <row r="69" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="B69" s="30"/>
+      <c r="C69" s="30"/>
+      <c r="D69" s="30"/>
+      <c r="E69" s="30"/>
+      <c r="F69" s="30"/>
+      <c r="G69" s="30"/>
+      <c r="H69" s="30"/>
+    </row>
+    <row r="70" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B70" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C70" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D70" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E70" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F70" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G70" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H70" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="15">
+        <v>1</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C71" s="2">
+        <v>100</v>
+      </c>
+      <c r="D71" s="2"/>
+      <c r="E71" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F71" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G71" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H71" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="15">
         <v>2</v>
       </c>
-      <c r="J13" s="36">
+      <c r="B72" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C72" s="2">
+        <v>101</v>
+      </c>
+      <c r="D72" s="2"/>
+      <c r="E72" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F72" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G72" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H72" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="16">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="31" t="s">
-        <v>60</v>
-      </c>
-      <c r="B15" s="31"/>
-      <c r="C15" s="31"/>
-      <c r="D15" s="31"/>
-      <c r="G15" s="31" t="s">
-        <v>67</v>
-      </c>
-      <c r="H15" s="31"/>
-      <c r="I15" s="31"/>
-      <c r="J15" s="31"/>
-      <c r="L15" s="31" t="s">
-        <v>68</v>
-      </c>
-      <c r="M15" s="31"/>
-      <c r="N15" s="31"/>
-      <c r="O15" s="31"/>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="35" t="s">
-        <v>56</v>
-      </c>
-      <c r="B16" s="35" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" s="35" t="s">
-        <v>1</v>
-      </c>
-      <c r="D16" s="35" t="s">
-        <v>57</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="J16" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="L16" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="M16" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="N16" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="O16" s="37" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="36">
-        <v>1</v>
-      </c>
-      <c r="B17" s="29">
-        <v>45597</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D17" s="30">
+      <c r="B73" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C73" s="10">
+        <v>102</v>
+      </c>
+      <c r="D73" s="10"/>
+      <c r="E73" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G17" s="2">
-        <v>1</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="I17" s="3"/>
-      <c r="J17" s="36">
-        <v>1</v>
-      </c>
-      <c r="L17" s="2">
-        <v>1</v>
-      </c>
-      <c r="M17" s="2">
-        <v>10</v>
-      </c>
-      <c r="N17" s="2">
-        <v>5</v>
-      </c>
-      <c r="O17" s="38">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="36">
-        <v>2</v>
-      </c>
-      <c r="B18" s="29">
-        <v>45598</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D18" s="30">
-        <v>45</v>
-      </c>
-      <c r="G18" s="2">
-        <v>2</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="I18" s="3"/>
-      <c r="J18" s="36"/>
-      <c r="L18" s="2">
-        <v>2</v>
-      </c>
-      <c r="M18" s="2">
-        <v>3</v>
-      </c>
-      <c r="N18" s="2">
-        <v>5</v>
-      </c>
-      <c r="O18" s="38">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="36">
-        <v>3</v>
-      </c>
-      <c r="B19" s="29">
-        <v>45600</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D19" s="30">
-        <v>110</v>
-      </c>
-      <c r="G19" s="2">
-        <v>3</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="I19" s="3"/>
-      <c r="J19" s="36"/>
-      <c r="L19" s="2">
-        <v>3</v>
-      </c>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
-      <c r="O19" s="38"/>
+      <c r="F73" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="G73" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="H73" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="43"/>
+      <c r="B74" s="44"/>
+      <c r="C74" s="43"/>
+      <c r="D74" s="43"/>
+      <c r="E74" s="43"/>
+      <c r="G74" s="43"/>
+      <c r="H74" s="43"/>
+    </row>
+    <row r="75" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="43"/>
+      <c r="B75" s="44"/>
+      <c r="C75" s="43"/>
+      <c r="D75" s="43"/>
+      <c r="E75" s="43"/>
+      <c r="G75" s="43"/>
+      <c r="H75" s="43"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="8">
+  <pageSetup paperSize="9" scale="58" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <tableParts count="12">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
@@ -3511,6 +5413,10 @@
     <tablePart r:id="rId7"/>
     <tablePart r:id="rId8"/>
     <tablePart r:id="rId9"/>
+    <tablePart r:id="rId10"/>
+    <tablePart r:id="rId11"/>
+    <tablePart r:id="rId12"/>
+    <tablePart r:id="rId13"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>